<commit_message>
aggiornamento test highpriority retail
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/test_Ind_High_Priority_RETAIL.xlsx
+++ b/earlywarning-pom/Document/test/test_Ind_High_Priority_RETAIL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="casistiche_indeterminate" sheetId="2" r:id="rId1"/>
     <sheet name="High_Priority" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="192">
   <si>
     <t>SNDG</t>
   </si>
@@ -561,13 +561,49 @@
   </si>
   <si>
     <t>FLG_JD_REATI_GRAVI_FAM</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>aggiungere il controllo num and den null</t>
+  </si>
+  <si>
+    <t>non trovo l'sndg nella CT</t>
+  </si>
+  <si>
+    <t>il 29 non è di tipologia flag ma un decimal(10,0)</t>
+  </si>
+  <si>
+    <t>FLG_ROTTURA_COVE</t>
+  </si>
+  <si>
+    <t>COVE_INIZIO_ROTTURA_DT</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Current Date</t>
+  </si>
+  <si>
+    <t>esito</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,8 +624,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,8 +652,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -632,11 +688,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -668,13 +744,51 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -992,19 +1106,19 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>37</v>
       </c>
@@ -1012,13 +1126,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>40</v>
       </c>
@@ -1026,55 +1140,55 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="13"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>50</v>
       </c>
@@ -1082,19 +1196,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>51</v>
@@ -1111,30 +1225,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L137"/>
+  <dimension ref="A1:P137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I134" sqref="I134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.42578125" customWidth="1"/>
+    <col min="14" max="14" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -1153,8 +1270,11 @@
       <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1164,11 +1284,18 @@
       <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1181,11 +1308,18 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1195,26 +1329,33 @@
       <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>0</v>
       </c>
@@ -1233,8 +1374,11 @@
       <c r="G9" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1244,11 +1388,18 @@
       <c r="D10" s="4">
         <v>0</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1261,11 +1412,18 @@
       <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1275,26 +1433,33 @@
       <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>0</v>
       </c>
@@ -1313,8 +1478,11 @@
       <c r="G16" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H16" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
@@ -1324,11 +1492,18 @@
       <c r="D17" s="4">
         <v>0</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1341,11 +1516,18 @@
       <c r="D18" s="4">
         <v>1</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
         <v>10</v>
@@ -1356,26 +1538,33 @@
       <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>0</v>
       </c>
@@ -1394,8 +1583,11 @@
       <c r="G23" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H23" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
@@ -1405,11 +1597,18 @@
       <c r="D24" s="4">
         <v>0</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -1422,11 +1621,18 @@
       <c r="D25" s="4">
         <v>1</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
       <c r="F25" s="4"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1436,16 +1642,23 @@
       <c r="D26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G26" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>0</v>
       </c>
@@ -1479,8 +1692,11 @@
       <c r="L30" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1506,11 +1722,16 @@
       <c r="I31" s="8">
         <v>800</v>
       </c>
-      <c r="J31" s="8"/>
+      <c r="J31" s="8">
+        <v>0.28571400000000002</v>
+      </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>20</v>
       </c>
@@ -1538,13 +1759,20 @@
       <c r="I32" s="8">
         <v>700</v>
       </c>
-      <c r="J32" s="8"/>
+      <c r="J32" s="8">
+        <v>100</v>
+      </c>
       <c r="K32" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L32" s="4"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>23</v>
       </c>
@@ -1569,13 +1797,20 @@
       <c r="I33" s="8">
         <v>0</v>
       </c>
-      <c r="J33" s="8"/>
+      <c r="J33" s="8">
+        <v>100</v>
+      </c>
       <c r="K33" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L33" s="4"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L33" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>58</v>
       </c>
@@ -1600,13 +1835,20 @@
       <c r="I34" s="8">
         <v>700</v>
       </c>
-      <c r="J34" s="8"/>
+      <c r="J34" s="8">
+        <v>0</v>
+      </c>
       <c r="K34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L34" s="4"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>59</v>
       </c>
@@ -1631,13 +1873,20 @@
       <c r="I35" s="8">
         <v>0</v>
       </c>
-      <c r="J35" s="8"/>
+      <c r="J35" s="8">
+        <v>0</v>
+      </c>
       <c r="K35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L35" s="4"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>60</v>
       </c>
@@ -1662,13 +1911,20 @@
       <c r="I36" s="8">
         <v>-10</v>
       </c>
-      <c r="J36" s="8"/>
+      <c r="J36" s="15">
+        <v>-1000000</v>
+      </c>
       <c r="K36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L36" s="4"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>61</v>
       </c>
@@ -1693,13 +1949,20 @@
       <c r="I37" s="8">
         <v>0</v>
       </c>
-      <c r="J37" s="8"/>
+      <c r="J37" s="15">
+        <v>-1000000</v>
+      </c>
       <c r="K37" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L37" s="4"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>62</v>
       </c>
@@ -1724,13 +1987,20 @@
       <c r="I38" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J38" s="8"/>
+      <c r="J38" s="15">
+        <v>-1000000</v>
+      </c>
       <c r="K38" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L38" s="4"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>63</v>
       </c>
@@ -1755,13 +2025,20 @@
       <c r="I39" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J39" s="8"/>
+      <c r="J39" s="15">
+        <v>-1000000</v>
+      </c>
       <c r="K39" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L39" s="4"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>64</v>
       </c>
@@ -1786,14 +2063,21 @@
       <c r="I40" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J40" s="8"/>
+      <c r="J40" s="15">
+        <v>-1000000</v>
+      </c>
       <c r="K40" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L40" s="4"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B41" s="14" t="s">
+      <c r="L40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -1817,13 +2101,18 @@
       <c r="I41" s="8">
         <v>700</v>
       </c>
-      <c r="J41" s="8"/>
+      <c r="J41" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="K41" s="4" t="s">
         <v>57</v>
       </c>
       <c r="L41" s="4"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
         <v>0</v>
       </c>
@@ -1842,8 +2131,11 @@
       <c r="G44" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H44" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>92</v>
       </c>
@@ -1853,13 +2145,20 @@
       <c r="D45" s="4">
         <v>0</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E45" s="4">
+        <v>0</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>67</v>
       </c>
@@ -1872,13 +2171,20 @@
       <c r="D46" s="4">
         <v>1</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G46" s="8"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E46" s="4">
+        <v>1</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>94</v>
       </c>
@@ -1888,13 +2194,20 @@
       <c r="D47" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
         <v>0</v>
       </c>
@@ -1913,8 +2226,11 @@
       <c r="G50" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>95</v>
       </c>
@@ -1924,11 +2240,18 @@
       <c r="D51" s="4">
         <v>0</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4">
+        <v>0</v>
+      </c>
       <c r="F51" s="4"/>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G51" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>71</v>
       </c>
@@ -1941,11 +2264,18 @@
       <c r="D52" s="4">
         <v>1</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4">
+        <v>1</v>
+      </c>
       <c r="F52" s="4"/>
-      <c r="G52" s="8"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>97</v>
       </c>
@@ -1955,13 +2285,20 @@
       <c r="D53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F53" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G53" s="11"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G53" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" s="12" t="s">
         <v>0</v>
       </c>
@@ -1980,8 +2317,11 @@
       <c r="G56" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>98</v>
       </c>
@@ -1991,13 +2331,20 @@
       <c r="D57" s="4">
         <v>0</v>
       </c>
-      <c r="E57" s="4"/>
+      <c r="E57" s="4">
+        <v>0</v>
+      </c>
       <c r="F57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="8"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>77</v>
       </c>
@@ -2010,13 +2357,20 @@
       <c r="D58" s="4">
         <v>1</v>
       </c>
-      <c r="E58" s="4"/>
+      <c r="E58" s="4">
+        <v>1</v>
+      </c>
       <c r="F58" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="8"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>100</v>
       </c>
@@ -2026,13 +2380,23 @@
       <c r="D59" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="4"/>
+      <c r="E59" s="4">
+        <v>0</v>
+      </c>
       <c r="F59" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="11"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G59" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H59" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I59" s="25"/>
+      <c r="J59" s="25"/>
+      <c r="K59" s="25"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="12" t="s">
         <v>0</v>
       </c>
@@ -2051,8 +2415,11 @@
       <c r="G62" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>101</v>
       </c>
@@ -2062,13 +2429,20 @@
       <c r="D63" s="4">
         <v>0</v>
       </c>
-      <c r="E63" s="4"/>
+      <c r="E63" s="4">
+        <v>0</v>
+      </c>
       <c r="F63" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G63" s="8"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G63" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>80</v>
       </c>
@@ -2081,13 +2455,20 @@
       <c r="D64" s="4">
         <v>1</v>
       </c>
-      <c r="E64" s="4"/>
+      <c r="E64" s="4">
+        <v>1</v>
+      </c>
       <c r="F64" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G64" s="8"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G64" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>103</v>
       </c>
@@ -2097,13 +2478,23 @@
       <c r="D65" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="E65" s="4">
+        <v>0</v>
+      </c>
       <c r="F65" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G65" s="11"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H65" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="25"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B68" s="12" t="s">
         <v>0</v>
       </c>
@@ -2122,8 +2513,11 @@
       <c r="G68" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>104</v>
       </c>
@@ -2137,9 +2531,16 @@
       <c r="F69" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G69" s="8"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G69" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H69" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="I69" s="20"/>
+      <c r="J69" s="20"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>84</v>
       </c>
@@ -2152,13 +2553,20 @@
       <c r="D70" s="4">
         <v>1</v>
       </c>
-      <c r="E70" s="4"/>
+      <c r="E70" s="4">
+        <v>1</v>
+      </c>
       <c r="F70" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="8"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G70" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
         <v>106</v>
       </c>
@@ -2168,13 +2576,23 @@
       <c r="D71" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E71" s="4"/>
+      <c r="E71" s="4">
+        <v>0</v>
+      </c>
       <c r="F71" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G71" s="11"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G71" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H71" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="I71" s="25"/>
+      <c r="J71" s="25"/>
+      <c r="K71" s="25"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B74" s="12" t="s">
         <v>0</v>
       </c>
@@ -2193,8 +2611,11 @@
       <c r="G74" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>107</v>
       </c>
@@ -2204,13 +2625,22 @@
       <c r="D75" s="4">
         <v>0</v>
       </c>
-      <c r="E75" s="4"/>
+      <c r="E75" s="4">
+        <v>0</v>
+      </c>
       <c r="F75" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G75" s="8"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G75" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>88</v>
       </c>
@@ -2223,13 +2653,20 @@
       <c r="D76" s="4">
         <v>1</v>
       </c>
-      <c r="E76" s="4"/>
+      <c r="E76" s="4">
+        <v>1</v>
+      </c>
       <c r="F76" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G76" s="8"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G76" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
         <v>109</v>
       </c>
@@ -2239,13 +2676,23 @@
       <c r="D77" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="4"/>
+      <c r="E77" s="4">
+        <v>0</v>
+      </c>
       <c r="F77" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G77" s="11"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G77" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H77" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I77" s="25"/>
+      <c r="J77" s="25"/>
+      <c r="K77" s="25"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B80" s="12" t="s">
         <v>0</v>
       </c>
@@ -2264,8 +2711,11 @@
       <c r="G80" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H80" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>113</v>
       </c>
@@ -2275,13 +2725,20 @@
       <c r="D81" s="4">
         <v>0</v>
       </c>
-      <c r="E81" s="4"/>
+      <c r="E81" s="4">
+        <v>0</v>
+      </c>
       <c r="F81" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="8"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G81" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>110</v>
       </c>
@@ -2294,13 +2751,20 @@
       <c r="D82" s="4">
         <v>1</v>
       </c>
-      <c r="E82" s="4"/>
+      <c r="E82" s="4">
+        <v>1</v>
+      </c>
       <c r="F82" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G82" s="8"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G82" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
         <v>115</v>
       </c>
@@ -2310,13 +2774,20 @@
       <c r="D83" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E83" s="4"/>
+      <c r="E83" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F83" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G83" s="11"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G83" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B86" s="12" t="s">
         <v>0</v>
       </c>
@@ -2335,8 +2806,11 @@
       <c r="G86" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H86" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
         <v>118</v>
       </c>
@@ -2346,13 +2820,20 @@
       <c r="D87" s="4">
         <v>0</v>
       </c>
-      <c r="E87" s="4"/>
+      <c r="E87" s="4">
+        <v>0</v>
+      </c>
       <c r="F87" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G87" s="8"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G87" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>121</v>
       </c>
@@ -2365,13 +2846,20 @@
       <c r="D88" s="4">
         <v>1</v>
       </c>
-      <c r="E88" s="4"/>
+      <c r="E88" s="4">
+        <v>1</v>
+      </c>
       <c r="F88" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G88" s="8"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G88" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
         <v>120</v>
       </c>
@@ -2381,13 +2869,20 @@
       <c r="D89" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E89" s="4"/>
+      <c r="E89" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F89" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G89" s="11"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G89" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B92" s="12" t="s">
         <v>0</v>
       </c>
@@ -2406,8 +2901,11 @@
       <c r="G92" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H92" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
         <v>127</v>
       </c>
@@ -2417,13 +2915,22 @@
       <c r="D93" s="4">
         <v>0</v>
       </c>
-      <c r="E93" s="4"/>
+      <c r="E93" s="4">
+        <v>0</v>
+      </c>
       <c r="F93" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G93" s="8"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G93" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I93" s="17"/>
+      <c r="J93" s="17"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>124</v>
       </c>
@@ -2436,13 +2943,20 @@
       <c r="D94" s="4">
         <v>1</v>
       </c>
-      <c r="E94" s="4"/>
+      <c r="E94" s="4">
+        <v>1</v>
+      </c>
       <c r="F94" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G94" s="8"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G94" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
         <v>129</v>
       </c>
@@ -2452,13 +2966,23 @@
       <c r="D95" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E95" s="4"/>
+      <c r="E95" s="4">
+        <v>0</v>
+      </c>
       <c r="F95" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G95" s="11"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G95" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H95" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I95" s="25"/>
+      <c r="J95" s="25"/>
+      <c r="K95" s="25"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B98" s="12" t="s">
         <v>0</v>
       </c>
@@ -2477,8 +3001,11 @@
       <c r="G98" s="4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H98" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>134</v>
       </c>
@@ -2488,13 +3015,22 @@
       <c r="D99" s="4">
         <v>0</v>
       </c>
-      <c r="E99" s="4"/>
+      <c r="E99" s="4">
+        <v>0</v>
+      </c>
       <c r="F99" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G99" s="8"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G99" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I99" s="17"/>
+      <c r="J99" s="17"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>131</v>
       </c>
@@ -2507,13 +3043,20 @@
       <c r="D100" s="4">
         <v>1</v>
       </c>
-      <c r="E100" s="4"/>
+      <c r="E100" s="4">
+        <v>1</v>
+      </c>
       <c r="F100" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G100" s="8"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G100" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
         <v>136</v>
       </c>
@@ -2523,13 +3066,23 @@
       <c r="D101" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E101" s="4"/>
+      <c r="E101" s="4">
+        <v>0</v>
+      </c>
       <c r="F101" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G101" s="11"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G101" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H101" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I101" s="25"/>
+      <c r="J101" s="25"/>
+      <c r="K101" s="25"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B104" s="12" t="s">
         <v>0</v>
       </c>
@@ -2548,8 +3101,11 @@
       <c r="G104" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H104" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>141</v>
       </c>
@@ -2559,13 +3115,22 @@
       <c r="D105" s="4">
         <v>0</v>
       </c>
-      <c r="E105" s="4"/>
+      <c r="E105" s="4">
+        <v>0</v>
+      </c>
       <c r="F105" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G105" s="8"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G105" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I105" s="17"/>
+      <c r="J105" s="17"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>138</v>
       </c>
@@ -2578,13 +3143,20 @@
       <c r="D106" s="4">
         <v>1</v>
       </c>
-      <c r="E106" s="4"/>
+      <c r="E106" s="4">
+        <v>1</v>
+      </c>
       <c r="F106" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G106" s="8"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G106" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B107" s="5" t="s">
         <v>143</v>
       </c>
@@ -2594,13 +3166,23 @@
       <c r="D107" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E107" s="4"/>
+      <c r="E107" s="4">
+        <v>0</v>
+      </c>
       <c r="F107" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G107" s="11"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G107" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H107" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I107" s="25"/>
+      <c r="J107" s="25"/>
+      <c r="K107" s="25"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B110" s="12" t="s">
         <v>0</v>
       </c>
@@ -2619,8 +3201,11 @@
       <c r="G110" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H110" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
         <v>148</v>
       </c>
@@ -2630,13 +3215,22 @@
       <c r="D111" s="4">
         <v>0</v>
       </c>
-      <c r="E111" s="4"/>
+      <c r="E111" s="4">
+        <v>0</v>
+      </c>
       <c r="F111" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G111" s="8"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G111" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I111" s="17"/>
+      <c r="J111" s="17"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>145</v>
       </c>
@@ -2649,13 +3243,20 @@
       <c r="D112" s="4">
         <v>1</v>
       </c>
-      <c r="E112" s="4"/>
+      <c r="E112" s="4">
+        <v>1</v>
+      </c>
       <c r="F112" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G112" s="8"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G112" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
         <v>150</v>
       </c>
@@ -2665,13 +3266,23 @@
       <c r="D113" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E113" s="4"/>
+      <c r="E113" s="4">
+        <v>0</v>
+      </c>
       <c r="F113" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G113" s="11"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G113" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H113" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I113" s="25"/>
+      <c r="J113" s="25"/>
+      <c r="K113" s="25"/>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B116" s="12" t="s">
         <v>0</v>
       </c>
@@ -2690,8 +3301,11 @@
       <c r="G116" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H116" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
         <v>153</v>
       </c>
@@ -2706,8 +3320,29 @@
         <v>5</v>
       </c>
       <c r="G117" s="8"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H117" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="I117" s="19"/>
+      <c r="J117" s="19"/>
+      <c r="K117" s="19"/>
+      <c r="L117" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="M117" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="N117" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="O117" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="P117" s="24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>152</v>
       </c>
@@ -2725,8 +3360,23 @@
         <v>5</v>
       </c>
       <c r="G118" s="8"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L118" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="M118" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="N118" s="21">
+        <v>42810</v>
+      </c>
+      <c r="O118" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="P118" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
         <v>155</v>
       </c>
@@ -2741,8 +3391,40 @@
         <v>5</v>
       </c>
       <c r="G119" s="11"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L119" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="M119" s="21">
+        <v>42735</v>
+      </c>
+      <c r="N119" s="21">
+        <v>42810</v>
+      </c>
+      <c r="O119" s="22">
+        <v>9085</v>
+      </c>
+      <c r="P119" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L120" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="M120" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="N120" s="21">
+        <v>42810</v>
+      </c>
+      <c r="O120" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="P120" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B122" s="12" t="s">
         <v>0</v>
       </c>
@@ -2761,8 +3443,11 @@
       <c r="G122" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H122" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B123" s="5" t="s">
         <v>165</v>
       </c>
@@ -2772,13 +3457,20 @@
       <c r="D123" s="4">
         <v>0</v>
       </c>
-      <c r="E123" s="4"/>
+      <c r="E123" s="4">
+        <v>0</v>
+      </c>
       <c r="F123" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G123" s="8"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G123" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>159</v>
       </c>
@@ -2791,13 +3483,20 @@
       <c r="D124" s="4">
         <v>1</v>
       </c>
-      <c r="E124" s="4"/>
+      <c r="E124" s="4">
+        <v>1</v>
+      </c>
       <c r="F124" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G124" s="8"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G124" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B125" s="5" t="s">
         <v>167</v>
       </c>
@@ -2807,13 +3506,23 @@
       <c r="D125" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E125" s="4"/>
+      <c r="E125" s="4">
+        <v>0</v>
+      </c>
       <c r="F125" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G125" s="11"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G125" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H125" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I125" s="25"/>
+      <c r="J125" s="25"/>
+      <c r="K125" s="25"/>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B128" s="12" t="s">
         <v>0</v>
       </c>
@@ -2832,8 +3541,11 @@
       <c r="G128" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H128" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" s="5" t="s">
         <v>168</v>
       </c>
@@ -2843,13 +3555,20 @@
       <c r="D129" s="4">
         <v>0</v>
       </c>
-      <c r="E129" s="4"/>
+      <c r="E129" s="4">
+        <v>0</v>
+      </c>
       <c r="F129" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G129" s="8"/>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G129" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>164</v>
       </c>
@@ -2862,13 +3581,20 @@
       <c r="D130" s="4">
         <v>1</v>
       </c>
-      <c r="E130" s="4"/>
+      <c r="E130" s="4">
+        <v>1</v>
+      </c>
       <c r="F130" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G130" s="8"/>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G130" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B131" s="5" t="s">
         <v>170</v>
       </c>
@@ -2878,13 +3604,20 @@
       <c r="D131" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E131" s="4"/>
+      <c r="E131" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F131" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G131" s="11"/>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G131" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B134" s="12" t="s">
         <v>0</v>
       </c>
@@ -2903,8 +3636,11 @@
       <c r="G134" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H134" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B135" s="5" t="s">
         <v>174</v>
       </c>
@@ -2914,13 +3650,20 @@
       <c r="D135" s="4">
         <v>0</v>
       </c>
-      <c r="E135" s="4"/>
+      <c r="E135" s="4">
+        <v>0</v>
+      </c>
       <c r="F135" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G135" s="8"/>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G135" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>171</v>
       </c>
@@ -2933,13 +3676,20 @@
       <c r="D136" s="4">
         <v>1</v>
       </c>
-      <c r="E136" s="4"/>
+      <c r="E136" s="4">
+        <v>1</v>
+      </c>
       <c r="F136" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G136" s="8"/>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G136" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B137" s="5" t="s">
         <v>176</v>
       </c>
@@ -2949,13 +3699,24 @@
       <c r="D137" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E137" s="4"/>
+      <c r="E137" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F137" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G137" s="11"/>
+      <c r="G137" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>190</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H69:J69"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiornamento ind esperenziali e test retail
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/test_Ind_High_Priority_RETAIL.xlsx
+++ b/earlywarning-pom/Document/test/test_Ind_High_Priority_RETAIL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="casistiche_indeterminate" sheetId="2" r:id="rId1"/>
     <sheet name="High_Priority" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="190">
   <si>
     <t>SNDG</t>
   </si>
@@ -585,12 +585,18 @@
   </si>
   <si>
     <t>0000000000000072</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>non trovo nessun l'sndg valorizzato in quel modo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -621,7 +627,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,6 +643,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -737,9 +749,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -776,9 +785,27 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1096,19 +1123,19 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="20"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="34"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>37</v>
       </c>
@@ -1116,13 +1143,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>40</v>
       </c>
@@ -1130,55 +1157,55 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="20"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="34"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>50</v>
       </c>
@@ -1186,19 +1213,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>51</v>
@@ -1217,31 +1244,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="25.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="25.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.44140625" customWidth="1"/>
-    <col min="14" max="14" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.42578125" customWidth="1"/>
+    <col min="14" max="14" width="50.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -1260,11 +1287,11 @@
       <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1285,7 +1312,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1309,7 +1336,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1319,27 +1346,31 @@
       <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>0</v>
       </c>
@@ -1358,11 +1389,11 @@
       <c r="G9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1383,7 +1414,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1407,7 +1438,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1417,27 +1448,31 @@
       <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>0</v>
       </c>
@@ -1456,11 +1491,11 @@
       <c r="G16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
@@ -1481,7 +1516,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1505,7 +1540,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
         <v>10</v>
@@ -1516,27 +1551,31 @@
       <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H19" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>0</v>
       </c>
@@ -1555,11 +1594,11 @@
       <c r="G23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
@@ -1580,7 +1619,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -1604,7 +1643,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1614,17 +1653,21 @@
       <c r="D26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H26" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>0</v>
       </c>
@@ -1658,11 +1701,14 @@
       <c r="L30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M30" s="29" t="s">
+      <c r="M30" s="28" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30" s="41" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1699,37 +1745,37 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="23">
+      <c r="C32" s="22">
         <v>100</v>
       </c>
-      <c r="D32" s="21">
-        <v>0</v>
-      </c>
-      <c r="E32" s="23">
+      <c r="D32" s="20">
+        <v>0</v>
+      </c>
+      <c r="E32" s="22">
         <v>1000</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="22">
         <v>700</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="22">
         <v>600</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="22">
         <f t="shared" ref="H32:H38" si="0">D32-E32</f>
         <v>-1000</v>
       </c>
-      <c r="I32" s="23">
+      <c r="I32" s="22">
         <f t="shared" ref="I32:I37" si="1">MAX(F32,G32)</f>
         <v>700</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="22">
         <v>100</v>
       </c>
       <c r="K32" s="4" t="s">
@@ -1742,7 +1788,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>23</v>
       </c>
@@ -1775,19 +1821,21 @@
       <c r="K33" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L33" s="30" t="s">
+      <c r="L33" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="M33" s="8"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M33" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="4">
         <v>0</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="20">
         <v>1000</v>
       </c>
       <c r="E34" s="8">
@@ -1813,21 +1861,21 @@
       <c r="K34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L34" s="30" t="s">
+      <c r="L34" s="29" t="s">
         <v>56</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C35" s="4">
         <v>0</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="20">
         <v>1000</v>
       </c>
       <c r="E35" s="8">
@@ -1853,21 +1901,21 @@
       <c r="K35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L35" s="30" t="s">
+      <c r="L35" s="29" t="s">
         <v>56</v>
       </c>
       <c r="M35" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="20">
         <v>1000</v>
       </c>
       <c r="E36" s="8">
@@ -1893,37 +1941,37 @@
       <c r="K36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L36" s="30" t="s">
+      <c r="L36" s="29" t="s">
         <v>57</v>
       </c>
       <c r="M36" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B37" s="5" t="s">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="1">
+      <c r="C37" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="36">
         <v>600</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="37">
         <v>600</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="38">
         <v>-10</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="38">
         <v>-70</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="38">
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
@@ -1931,15 +1979,18 @@
         <v>57</v>
       </c>
       <c r="M37" s="6"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N37" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="20">
         <v>-1000</v>
       </c>
       <c r="E38" s="8">
@@ -1965,21 +2016,21 @@
       <c r="K38" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L38" s="30" t="s">
+      <c r="L38" s="29" t="s">
         <v>57</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="20">
         <v>1000</v>
       </c>
       <c r="E39" s="8">
@@ -2004,14 +2055,14 @@
       <c r="K39" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L39" s="30" t="s">
+      <c r="L39" s="29" t="s">
         <v>57</v>
       </c>
       <c r="M39" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>64</v>
       </c>
@@ -2042,14 +2093,14 @@
       <c r="K40" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="29" t="s">
         <v>57</v>
       </c>
       <c r="M40" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>66</v>
       </c>
@@ -2080,14 +2131,14 @@
       <c r="K41" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="29" t="s">
         <v>57</v>
       </c>
       <c r="M41" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>92</v>
       </c>
@@ -2118,18 +2169,18 @@
       <c r="K42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L42" s="30" t="s">
+      <c r="L42" s="29" t="s">
         <v>57</v>
       </c>
       <c r="M42" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -2151,36 +2202,42 @@
         <f>MAX(F43,G43)</f>
         <v>700</v>
       </c>
-      <c r="J43" s="8"/>
+      <c r="J43" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="K43" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L43" s="30"/>
-      <c r="M43" s="8"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B44" s="13" t="s">
+      <c r="L43" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="C44" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="38">
         <v>-10</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="38">
         <v>-70</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="38">
         <f>MAX(F44,G44)</f>
         <v>-10</v>
       </c>
@@ -2188,32 +2245,35 @@
       <c r="K44" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L44" s="30"/>
+      <c r="L44" s="29"/>
       <c r="M44" s="8"/>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B45" s="13" t="s">
+      <c r="N44" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B45" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="4" t="s">
+      <c r="C45" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="8">
-        <v>0</v>
-      </c>
-      <c r="G45" s="8">
+      <c r="F45" s="38">
+        <v>0</v>
+      </c>
+      <c r="G45" s="38">
         <v>-30</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H45" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="38">
         <f>MAX(F45,G45)</f>
         <v>0</v>
       </c>
@@ -2221,24 +2281,30 @@
       <c r="K45" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L45" s="30"/>
-      <c r="M45" s="23"/>
-    </row>
-    <row r="46" spans="2:13" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="26"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="28"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L45" s="29"/>
+      <c r="M45" s="22"/>
+      <c r="N45" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="25"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="27"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="12" t="s">
         <v>0</v>
       </c>
@@ -2257,11 +2323,11 @@
       <c r="G48" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H48" s="29" t="s">
+      <c r="H48" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>96</v>
       </c>
@@ -2282,7 +2348,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>67</v>
       </c>
@@ -2306,7 +2372,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>98</v>
       </c>
@@ -2316,14 +2382,21 @@
       <c r="D51" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4">
+        <v>0</v>
+      </c>
       <c r="F51" s="8"/>
       <c r="G51" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H51" s="8"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H51" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
         <v>0</v>
       </c>
@@ -2342,11 +2415,11 @@
       <c r="G54" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H54" s="29" t="s">
+      <c r="H54" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>99</v>
       </c>
@@ -2367,7 +2440,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>71</v>
       </c>
@@ -2391,7 +2464,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>101</v>
       </c>
@@ -2401,16 +2474,20 @@
       <c r="D57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="4"/>
+      <c r="E57" s="4">
+        <v>0</v>
+      </c>
       <c r="F57" s="10" t="s">
         <v>75</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H57" s="8"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H57" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" s="12" t="s">
         <v>0</v>
       </c>
@@ -2429,11 +2506,11 @@
       <c r="G60" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H60" s="29" t="s">
+      <c r="H60" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>102</v>
       </c>
@@ -2454,7 +2531,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>77</v>
       </c>
@@ -2478,27 +2555,31 @@
         <v>179</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C63" s="21">
+      <c r="C63" s="20">
         <v>0</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E63" s="4"/>
+      <c r="E63" s="4">
+        <v>0</v>
+      </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H63" s="8"/>
+      <c r="H63" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I63" s="19"/>
       <c r="J63" s="19"/>
       <c r="K63" s="19"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B66" s="12" t="s">
         <v>0</v>
       </c>
@@ -2517,11 +2598,11 @@
       <c r="G66" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H66" s="29" t="s">
+      <c r="H66" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>104</v>
       </c>
@@ -2542,7 +2623,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>80</v>
       </c>
@@ -2566,7 +2647,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>106</v>
       </c>
@@ -2576,17 +2657,21 @@
       <c r="D69" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E69" s="4"/>
+      <c r="E69" s="4">
+        <v>0</v>
+      </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H69" s="8"/>
+      <c r="H69" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I69" s="19"/>
       <c r="J69" s="19"/>
       <c r="K69" s="19"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B72" s="12" t="s">
         <v>0</v>
       </c>
@@ -2605,12 +2690,12 @@
       <c r="G72" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H72" s="29" t="s">
+      <c r="H72" s="28" t="s">
         <v>183</v>
       </c>
       <c r="I72" s="15"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
         <v>107</v>
       </c>
@@ -2627,10 +2712,12 @@
       <c r="G73" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H73" s="8"/>
-      <c r="I73" s="31"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H73" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I73" s="30"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>84</v>
       </c>
@@ -2650,9 +2737,11 @@
       <c r="G74" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H74" s="8"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H74" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>112</v>
       </c>
@@ -2669,15 +2758,17 @@
       <c r="G75" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H75" s="8"/>
+      <c r="H75" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I75" s="19"/>
       <c r="K75" s="19"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I76" s="24"/>
-      <c r="J76" s="28"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I76" s="23"/>
+      <c r="J76" s="27"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B78" s="12" t="s">
         <v>0</v>
       </c>
@@ -2696,11 +2787,11 @@
       <c r="G78" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H78" s="29" t="s">
+      <c r="H78" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>113</v>
       </c>
@@ -2723,7 +2814,7 @@
       <c r="I79" s="16"/>
       <c r="J79" s="16"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>88</v>
       </c>
@@ -2747,7 +2838,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>117</v>
       </c>
@@ -2764,12 +2855,14 @@
       <c r="G81" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H81" s="8"/>
+      <c r="H81" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I81" s="19"/>
       <c r="J81" s="19"/>
       <c r="K81" s="19"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B84" s="12" t="s">
         <v>0</v>
       </c>
@@ -2788,11 +2881,11 @@
       <c r="G84" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H84" s="29" t="s">
+      <c r="H84" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
         <v>118</v>
       </c>
@@ -2813,7 +2906,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>109</v>
       </c>
@@ -2837,7 +2930,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
         <v>126</v>
       </c>
@@ -2847,14 +2940,18 @@
       <c r="D87" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E87" s="4"/>
+      <c r="E87" s="4">
+        <v>0</v>
+      </c>
       <c r="F87" s="4"/>
       <c r="G87" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H87" s="8"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H87" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B90" s="12" t="s">
         <v>0</v>
       </c>
@@ -2873,11 +2970,11 @@
       <c r="G90" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H90" s="29" t="s">
+      <c r="H90" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
         <v>127</v>
       </c>
@@ -2898,7 +2995,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>120</v>
       </c>
@@ -2922,7 +3019,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
         <v>133</v>
       </c>
@@ -2932,14 +3029,18 @@
       <c r="D93" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E93" s="4"/>
+      <c r="E93" s="4">
+        <v>0</v>
+      </c>
       <c r="F93" s="4"/>
       <c r="G93" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H93" s="8"/>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H93" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B96" s="12" t="s">
         <v>0</v>
       </c>
@@ -2958,11 +3059,11 @@
       <c r="G96" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H96" s="29" t="s">
+      <c r="H96" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
         <v>134</v>
       </c>
@@ -2985,7 +3086,7 @@
       <c r="I97" s="16"/>
       <c r="J97" s="16"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>123</v>
       </c>
@@ -3009,7 +3110,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>140</v>
       </c>
@@ -3019,17 +3120,21 @@
       <c r="D99" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E99" s="4"/>
+      <c r="E99" s="4">
+        <v>0</v>
+      </c>
       <c r="F99" s="4"/>
       <c r="G99" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H99" s="8"/>
+      <c r="H99" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I99" s="19"/>
       <c r="J99" s="19"/>
       <c r="K99" s="19"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B102" s="12" t="s">
         <v>0</v>
       </c>
@@ -3048,11 +3153,11 @@
       <c r="G102" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H102" s="29" t="s">
+      <c r="H102" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
         <v>141</v>
       </c>
@@ -3075,7 +3180,7 @@
       <c r="I103" s="16"/>
       <c r="J103" s="16"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>130</v>
       </c>
@@ -3099,7 +3204,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>147</v>
       </c>
@@ -3109,17 +3214,21 @@
       <c r="D105" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E105" s="4"/>
+      <c r="E105" s="4">
+        <v>0</v>
+      </c>
       <c r="F105" s="4"/>
       <c r="G105" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H105" s="8"/>
+      <c r="H105" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I105" s="19"/>
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B108" s="12" t="s">
         <v>0</v>
       </c>
@@ -3138,11 +3247,11 @@
       <c r="G108" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H108" s="29" t="s">
+      <c r="H108" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B109" s="5" t="s">
         <v>148</v>
       </c>
@@ -3165,7 +3274,7 @@
       <c r="I109" s="16"/>
       <c r="J109" s="16"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>137</v>
       </c>
@@ -3189,7 +3298,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
         <v>152</v>
       </c>
@@ -3199,17 +3308,21 @@
       <c r="D111" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E111" s="4"/>
+      <c r="E111" s="4">
+        <v>0</v>
+      </c>
       <c r="F111" s="4"/>
       <c r="G111" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H111" s="8"/>
+      <c r="H111" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I111" s="19"/>
       <c r="J111" s="19"/>
       <c r="K111" s="19"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B114" s="12" t="s">
         <v>0</v>
       </c>
@@ -3228,11 +3341,11 @@
       <c r="G114" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="H114" s="29" t="s">
+      <c r="H114" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
         <v>153</v>
       </c>
@@ -3255,7 +3368,7 @@
       <c r="I115" s="16"/>
       <c r="J115" s="16"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>144</v>
       </c>
@@ -3279,7 +3392,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
         <v>163</v>
       </c>
@@ -3289,30 +3402,34 @@
       <c r="D117" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E117" s="4"/>
+      <c r="E117" s="4">
+        <v>0</v>
+      </c>
       <c r="F117" s="4"/>
       <c r="G117" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H117" s="8"/>
+      <c r="H117" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I117" s="19"/>
       <c r="J117" s="19"/>
       <c r="K117" s="19"/>
     </row>
-    <row r="120" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C120" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D120" s="22" t="s">
+      <c r="D120" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="E120" s="22" t="s">
+      <c r="E120" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="F120" s="22" t="s">
+      <c r="F120" s="21" t="s">
         <v>182</v>
       </c>
       <c r="G120" s="4" t="s">
@@ -3324,13 +3441,13 @@
       <c r="I120" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="J120" s="29" t="s">
+      <c r="J120" s="28" t="s">
         <v>183</v>
       </c>
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B121" s="5" t="s">
         <v>164</v>
       </c>
@@ -3351,11 +3468,13 @@
         <v>5</v>
       </c>
       <c r="I121" s="8"/>
-      <c r="J121" s="8"/>
+      <c r="J121" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="K121" s="17"/>
       <c r="L121" s="17"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>151</v>
       </c>
@@ -3380,11 +3499,13 @@
         <v>5</v>
       </c>
       <c r="I122" s="8"/>
-      <c r="J122" s="8"/>
+      <c r="J122" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B123" s="5" t="s">
         <v>166</v>
       </c>
@@ -3405,11 +3526,13 @@
         <v>5</v>
       </c>
       <c r="I123" s="11"/>
-      <c r="J123" s="8"/>
+      <c r="J123" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B126" s="12" t="s">
         <v>0</v>
       </c>
@@ -3428,11 +3551,11 @@
       <c r="G126" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H126" s="29" t="s">
+      <c r="H126" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B127" s="5" t="s">
         <v>167</v>
       </c>
@@ -3453,7 +3576,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>157</v>
       </c>
@@ -3477,7 +3600,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B129" s="5" t="s">
         <v>172</v>
       </c>
@@ -3487,24 +3610,28 @@
       <c r="D129" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E129" s="4"/>
+      <c r="E129" s="4">
+        <v>0</v>
+      </c>
       <c r="F129" s="4"/>
       <c r="G129" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H129" s="8"/>
+      <c r="H129" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="I129" s="19"/>
       <c r="J129" s="19"/>
       <c r="K129" s="19"/>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K131" s="32"/>
-      <c r="L131" s="32"/>
-      <c r="M131" s="32"/>
-      <c r="N131" s="32"/>
-      <c r="O131" s="28"/>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K131" s="31"/>
+      <c r="L131" s="31"/>
+      <c r="M131" s="31"/>
+      <c r="N131" s="31"/>
+      <c r="O131" s="27"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B132" s="12" t="s">
         <v>0</v>
       </c>
@@ -3523,16 +3650,16 @@
       <c r="G132" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H132" s="29" t="s">
+      <c r="H132" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="K132" s="28"/>
-      <c r="L132" s="28"/>
-      <c r="M132" s="33"/>
-      <c r="N132" s="28"/>
-      <c r="O132" s="28"/>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K132" s="27"/>
+      <c r="L132" s="27"/>
+      <c r="M132" s="32"/>
+      <c r="N132" s="27"/>
+      <c r="O132" s="27"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B133" s="5" t="s">
         <v>173</v>
       </c>
@@ -3552,13 +3679,13 @@
       <c r="H133" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="K133" s="28"/>
-      <c r="L133" s="33"/>
-      <c r="M133" s="33"/>
-      <c r="N133" s="34"/>
-      <c r="O133" s="28"/>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K133" s="27"/>
+      <c r="L133" s="32"/>
+      <c r="M133" s="32"/>
+      <c r="N133" s="33"/>
+      <c r="O133" s="27"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>162</v>
       </c>
@@ -3581,13 +3708,13 @@
       <c r="H134" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="K134" s="28"/>
-      <c r="L134" s="28"/>
-      <c r="M134" s="33"/>
-      <c r="N134" s="28"/>
-      <c r="O134" s="28"/>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K134" s="27"/>
+      <c r="L134" s="27"/>
+      <c r="M134" s="32"/>
+      <c r="N134" s="27"/>
+      <c r="O134" s="27"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B135" s="5" t="s">
         <v>184</v>
       </c>
@@ -3597,14 +3724,18 @@
       <c r="D135" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E135" s="4"/>
+      <c r="E135" s="4">
+        <v>0</v>
+      </c>
       <c r="F135" s="4"/>
       <c r="G135" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H135" s="8"/>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H135" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B138" s="12" t="s">
         <v>0</v>
       </c>
@@ -3623,11 +3754,11 @@
       <c r="G138" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H138" s="29" t="s">
+      <c r="H138" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B139" s="5" t="s">
         <v>185</v>
       </c>
@@ -3648,7 +3779,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>169</v>
       </c>
@@ -3672,7 +3803,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B141" s="5" t="s">
         <v>187</v>
       </c>
@@ -3682,12 +3813,16 @@
       <c r="D141" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E141" s="4"/>
+      <c r="E141" s="4">
+        <v>0</v>
+      </c>
       <c r="F141" s="4"/>
       <c r="G141" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H141" s="8"/>
+      <c r="H141" s="8" t="s">
+        <v>179</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>